<commit_message>
Redid analysis as Bobby realized the initial data were totally wrong (data wrangling error early in bioinformatics steps). Did DR community occ model, updated NMDS, mean reads plot.
</commit_message>
<xml_diff>
--- a/data/Exxon Bat 2021.xlsx
+++ b/data/Exxon Bat 2021.xlsx
@@ -1,16 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\mike_files\Research\mammal\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8762371-6730-46F8-88AC-67A85236D327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sample Data" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Tree  Sample Data" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Metadata" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Data Sheet" sheetId="5" r:id="rId8"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Tree  Sample Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Metadata" sheetId="4" r:id="rId4"/>
+    <sheet name="Data Sheet" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -893,38 +913,41 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="m/d/yy"/>
-    <numFmt numFmtId="166" formatCode="m-d-yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yy"/>
+    <numFmt numFmtId="165" formatCode="m\-d\-yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFBCC0C3"/>
       <name val="Roboto"/>
     </font>
@@ -934,7 +957,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -956,86 +979,63 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1225,26 +1225,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="8" width="21.57"/>
+    <col min="1" max="8" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1253,27 +1256,28 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="28.0"/>
-    <col customWidth="1" min="3" max="3" width="30.0"/>
-    <col customWidth="1" min="5" max="5" width="19.86"/>
-    <col customWidth="1" min="7" max="7" width="25.71"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1302,9 +1306,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>44385.0</v>
+        <v>44385</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -1316,7 +1320,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="2">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
@@ -1325,9 +1329,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>44385.0</v>
+        <v>44385</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -1344,17 +1348,17 @@
       <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="str">
-        <f>IFS(F1:F100 = F3, "NA")</f>
-        <v>NA</v>
+      <c r="G3" s="2" t="e">
+        <f ca="1">_xludf.IFS(F1:F100 = F3, "NA")</f>
+        <v>#NAME?</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>44385.0</v>
+        <v>44385</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -1372,7 +1376,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="2">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
@@ -1381,9 +1385,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>44386.0</v>
+        <v>44386</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -1395,7 +1399,7 @@
         <v>11</v>
       </c>
       <c r="G5" s="2">
-        <v>325.0</v>
+        <v>325</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>13</v>
@@ -1404,9 +1408,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>44386.0</v>
+        <v>44386</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -1424,15 +1428,15 @@
         <v>22</v>
       </c>
       <c r="G6" s="2">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>44386.0</v>
+        <v>44386</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
@@ -1456,9 +1460,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>44386.0</v>
+        <v>44386</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>29</v>
@@ -1476,15 +1480,15 @@
         <v>22</v>
       </c>
       <c r="G8" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>44386.0</v>
+        <v>44386</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -1508,9 +1512,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>44387.0</v>
+        <v>44387</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>11</v>
@@ -1522,15 +1526,15 @@
         <v>11</v>
       </c>
       <c r="G10" s="2">
-        <v>146.0</v>
+        <v>146</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>44387.0</v>
+        <v>44387</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
@@ -1548,15 +1552,15 @@
         <v>22</v>
       </c>
       <c r="G11" s="2">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>44387.0</v>
+        <v>44387</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
@@ -1580,9 +1584,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>44387.0</v>
+        <v>44387</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>29</v>
@@ -1600,15 +1604,15 @@
         <v>22</v>
       </c>
       <c r="G13" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>44387.0</v>
+        <v>44387</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
@@ -1632,9 +1636,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>44387.0</v>
+        <v>44387</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>38</v>
@@ -1652,15 +1656,15 @@
         <v>22</v>
       </c>
       <c r="G15" s="2">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>44387.0</v>
+        <v>44387</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>38</v>
@@ -1684,9 +1688,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>41101.0</v>
+        <v>41101</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>11</v>
@@ -1698,15 +1702,15 @@
         <v>11</v>
       </c>
       <c r="G17" s="2">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>41101.0</v>
+        <v>41101</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>29</v>
@@ -1724,15 +1728,15 @@
         <v>22</v>
       </c>
       <c r="G18" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>41101.0</v>
+        <v>41101</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>29</v>
@@ -1756,9 +1760,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>41101.0</v>
+        <v>41101</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>38</v>
@@ -1776,15 +1780,15 @@
         <v>22</v>
       </c>
       <c r="G20" s="2">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>41101.0</v>
+        <v>41101</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>38</v>
@@ -1808,9 +1812,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>41101.0</v>
+        <v>41101</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>47</v>
@@ -1828,7 +1832,7 @@
         <v>22</v>
       </c>
       <c r="G22" s="2">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>13</v>
@@ -1837,9 +1841,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>41101.0</v>
+        <v>41101</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>47</v>
@@ -1863,9 +1867,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>44389.0</v>
+        <v>44389</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>11</v>
@@ -1877,19 +1881,19 @@
         <v>11</v>
       </c>
       <c r="G24" s="2">
-        <v>56.0</v>
-      </c>
-      <c r="H24" s="1" t="str">
-        <f>IFS(F1:F28 = "NC",H2,F1:F28 = "Soil", "Frozen @-20*",F1:F100 = "Roller", "ETOH &amp; -20*")</f>
-        <v>ETOH &amp; -20*</v>
+        <v>56</v>
+      </c>
+      <c r="H24" s="1" t="e">
+        <f ca="1">_xludf.IFS(F1:F28 = "NC",H2,F1:F28 = "Soil", "Frozen @-20*",F1:F100 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>44389.0</v>
+        <v>44389</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>38</v>
@@ -1907,16 +1911,16 @@
         <v>22</v>
       </c>
       <c r="G25" s="2">
-        <v>45.0</v>
-      </c>
-      <c r="H25" s="1" t="str">
-        <f t="shared" ref="H25:H29" si="1">IFS(F2:F29 = "NC",H3,F2:F29 = "Soil", "Frozen @-20*",F2:F102 = "Roller", "ETOH &amp; -20*")</f>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>45</v>
+      </c>
+      <c r="H25" s="1" t="e">
+        <f t="shared" ref="H25:H29" ca="1" si="0">_xludf.IFS(F2:F29 = "NC",H3,F2:F29 = "Soil", "Frozen @-20*",F2:F102 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>44389.0</v>
+        <v>44389</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>38</v>
@@ -1936,14 +1940,14 @@
       <c r="G26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="27">
+      <c r="H26" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>44389.0</v>
+        <v>44389</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>47</v>
@@ -1961,16 +1965,16 @@
         <v>22</v>
       </c>
       <c r="G27" s="2">
-        <v>126.0</v>
-      </c>
-      <c r="H27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>126</v>
+      </c>
+      <c r="H27" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>44389.0</v>
+        <v>44389</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>47</v>
@@ -1990,14 +1994,14 @@
       <c r="G28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H28" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="29">
+      <c r="H28" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>44390.0</v>
+        <v>44390</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>11</v>
@@ -2009,19 +2013,19 @@
         <v>11</v>
       </c>
       <c r="G29" s="2">
-        <v>86.0</v>
-      </c>
-      <c r="H29" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Frozen @ -20*</v>
+        <v>86</v>
+      </c>
+      <c r="H29" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>44390.0</v>
+        <v>44390</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>47</v>
@@ -2039,16 +2043,16 @@
         <v>22</v>
       </c>
       <c r="G30" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="H30" s="1" t="str">
-        <f t="shared" ref="H30:H65" si="2">IFS(F7:F34 = "NC",H8,F7:F34 = "Soil", "Frozen @-20*",F7:F106 = "Roller", "ETOH &amp; -20*")</f>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>40</v>
+      </c>
+      <c r="H30" s="1" t="e">
+        <f t="shared" ref="H30:H65" ca="1" si="1">_xludf.IFS(F7:F34 = "NC",H8,F7:F34 = "Soil", "Frozen @-20*",F7:F106 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>44390.0</v>
+        <v>44390</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>47</v>
@@ -2068,14 +2072,14 @@
       <c r="G31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="32">
+      <c r="H31" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>44391.0</v>
+        <v>44391</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>28</v>
@@ -2095,17 +2099,17 @@
       <c r="G32" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="H32" s="6" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>44392.0</v>
+        <v>44392</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>63</v>
@@ -2123,19 +2127,19 @@
         <v>22</v>
       </c>
       <c r="G33" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="H33" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
+        <v>30</v>
+      </c>
+      <c r="H33" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>44392.0</v>
+        <v>44392</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>63</v>
@@ -2155,14 +2159,14 @@
       <c r="G34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H34" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="35">
+      <c r="H34" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>44392.0</v>
+        <v>44392</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>11</v>
@@ -2174,16 +2178,16 @@
         <v>11</v>
       </c>
       <c r="G35" s="2">
-        <v>86.0</v>
-      </c>
-      <c r="H35" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>86</v>
+      </c>
+      <c r="H35" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>44392.0</v>
+        <v>44392</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>70</v>
@@ -2195,16 +2199,16 @@
         <v>22</v>
       </c>
       <c r="G36" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="H36" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>44392.0</v>
+        <v>44392</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>70</v>
@@ -2218,14 +2222,14 @@
       <c r="G37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H37" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="38">
+      <c r="H37" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>44392.0</v>
+        <v>44392</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>73</v>
@@ -2243,16 +2247,16 @@
         <v>22</v>
       </c>
       <c r="G38" s="2">
-        <v>36.0</v>
-      </c>
-      <c r="H38" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>36</v>
+      </c>
+      <c r="H38" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>44392.0</v>
+        <v>44392</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>73</v>
@@ -2272,17 +2276,17 @@
       <c r="G39" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H39" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
+      <c r="H39" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>44393.0</v>
+        <v>44393</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>11</v>
@@ -2294,19 +2298,19 @@
         <v>11</v>
       </c>
       <c r="G40" s="2">
-        <v>146.0</v>
-      </c>
-      <c r="H40" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
+        <v>146</v>
+      </c>
+      <c r="H40" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>44393.0</v>
+        <v>44393</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>63</v>
@@ -2324,19 +2328,19 @@
         <v>22</v>
       </c>
       <c r="G41" s="2">
-        <v>42.0</v>
-      </c>
-      <c r="H41" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
+        <v>42</v>
+      </c>
+      <c r="H41" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>44393.0</v>
+        <v>44393</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>63</v>
@@ -2356,14 +2360,14 @@
       <c r="G42" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H42" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="43">
+      <c r="H42" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>44393.0</v>
+        <v>44393</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>73</v>
@@ -2381,16 +2385,16 @@
         <v>22</v>
       </c>
       <c r="G43" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="H43" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>20</v>
+      </c>
+      <c r="H43" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>44393.0</v>
+        <v>44393</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>73</v>
@@ -2410,17 +2414,17 @@
       <c r="G44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H44" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
+      <c r="H44" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>44394.0</v>
+        <v>44394</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>11</v>
@@ -2432,19 +2436,19 @@
         <v>11</v>
       </c>
       <c r="G45" s="2">
-        <v>78.0</v>
-      </c>
-      <c r="H45" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @ -20*</v>
+        <v>78</v>
+      </c>
+      <c r="H45" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>44394.0</v>
+        <v>44394</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>63</v>
@@ -2462,16 +2466,16 @@
         <v>22</v>
       </c>
       <c r="G46" s="2">
-        <v>38.0</v>
-      </c>
-      <c r="H46" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>38</v>
+      </c>
+      <c r="H46" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>44394.0</v>
+        <v>44394</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>63</v>
@@ -2491,14 +2495,14 @@
       <c r="G47" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H47" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="48">
+      <c r="H47" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>44394.0</v>
+        <v>44394</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>73</v>
@@ -2516,19 +2520,19 @@
         <v>90</v>
       </c>
       <c r="G48" s="2">
-        <v>58.0</v>
-      </c>
-      <c r="H48" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
+        <v>58</v>
+      </c>
+      <c r="H48" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>44394.0</v>
+        <v>44394</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>73</v>
@@ -2548,14 +2552,14 @@
       <c r="G49" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H49" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="50">
+      <c r="H49" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>93</v>
@@ -2573,19 +2577,19 @@
         <v>22</v>
       </c>
       <c r="G50" s="2">
-        <v>95.0</v>
-      </c>
-      <c r="H50" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
+        <v>95</v>
+      </c>
+      <c r="H50" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>93</v>
@@ -2605,14 +2609,14 @@
       <c r="G51" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H51" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="52">
+      <c r="H51" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>99</v>
@@ -2630,19 +2634,19 @@
         <v>22</v>
       </c>
       <c r="G52" s="2">
-        <v>35.0</v>
-      </c>
-      <c r="H52" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
+        <v>35</v>
+      </c>
+      <c r="H52" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>104</v>
@@ -2662,14 +2666,14 @@
       <c r="G53" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H53" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="54">
+      <c r="H53" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>106</v>
@@ -2687,19 +2691,19 @@
         <v>22</v>
       </c>
       <c r="G54" s="2">
-        <v>145.0</v>
-      </c>
-      <c r="H54" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
+        <v>145</v>
+      </c>
+      <c r="H54" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>106</v>
@@ -2719,17 +2723,17 @@
       <c r="G55" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H55" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
+      <c r="H55" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>112</v>
@@ -2747,19 +2751,19 @@
         <v>22</v>
       </c>
       <c r="G56" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="H56" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
+        <v>80</v>
+      </c>
+      <c r="H56" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>112</v>
@@ -2779,17 +2783,17 @@
       <c r="G57" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H57" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
+      <c r="H57" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>11</v>
@@ -2801,16 +2805,16 @@
         <v>11</v>
       </c>
       <c r="G58" s="2">
-        <v>230.0</v>
-      </c>
-      <c r="H58" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>230</v>
+      </c>
+      <c r="H58" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>106</v>
@@ -2828,16 +2832,16 @@
         <v>22</v>
       </c>
       <c r="G59" s="2">
-        <v>110.0</v>
-      </c>
-      <c r="H59" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>110</v>
+      </c>
+      <c r="H59" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>106</v>
@@ -2854,14 +2858,14 @@
       <c r="F60" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H60" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="61">
+      <c r="H60" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>112</v>
@@ -2879,16 +2883,16 @@
         <v>22</v>
       </c>
       <c r="G61" s="2">
-        <v>130.0</v>
-      </c>
-      <c r="H61" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>130</v>
+      </c>
+      <c r="H61" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>112</v>
@@ -2905,14 +2909,14 @@
       <c r="F62" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H62" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="63">
+      <c r="H62" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>93</v>
@@ -2930,16 +2934,16 @@
         <v>22</v>
       </c>
       <c r="G63" s="2">
-        <v>70.0</v>
-      </c>
-      <c r="H63" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="64">
+        <v>70</v>
+      </c>
+      <c r="H63" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>93</v>
@@ -2956,14 +2960,14 @@
       <c r="F64" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H64" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="65">
+      <c r="H64" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>124</v>
@@ -2981,16 +2985,16 @@
         <v>22</v>
       </c>
       <c r="G65" s="2">
-        <v>210.0</v>
-      </c>
-      <c r="H65" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>210</v>
+      </c>
+      <c r="H65" s="1" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>124</v>
@@ -3007,14 +3011,14 @@
       <c r="F66" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H66" s="1" t="str">
-        <f>IFS(F43:F71 = "NC",H44,F43:F71 = "Soil", "Frozen @-20*",F43:F142 = "Roller", "ETOH &amp; -20*")</f>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="67">
+      <c r="H66" s="1" t="e">
+        <f ca="1">_xludf.IFS(F43:F71 = "NC",H44,F43:F71 = "Soil", "Frozen @-20*",F43:F142 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>99</v>
@@ -3032,16 +3036,16 @@
         <v>22</v>
       </c>
       <c r="G67" s="2">
-        <v>140.0</v>
-      </c>
-      <c r="H67" s="1" t="str">
-        <f t="shared" ref="H67:H92" si="3">IFS(F44:F71 = "NC",H45,F44:F71 = "Soil", "Frozen @-20*",F44:F143 = "Roller", "ETOH &amp; -20*")</f>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>140</v>
+      </c>
+      <c r="H67" s="1" t="e">
+        <f t="shared" ref="H67:H92" ca="1" si="2">_xludf.IFS(F44:F71 = "NC",H45,F44:F71 = "Soil", "Frozen @-20*",F44:F143 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>104</v>
@@ -3058,14 +3062,14 @@
       <c r="F68" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H68" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="69">
+      <c r="H68" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>130</v>
@@ -3083,16 +3087,16 @@
         <v>22</v>
       </c>
       <c r="G69" s="2">
-        <v>130.0</v>
-      </c>
-      <c r="H69" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>130</v>
+      </c>
+      <c r="H69" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>130</v>
@@ -3109,14 +3113,14 @@
       <c r="F70" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H70" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="71">
+      <c r="H70" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>11</v>
@@ -3128,16 +3132,16 @@
         <v>11</v>
       </c>
       <c r="G71" s="2">
-        <v>180.0</v>
-      </c>
-      <c r="H71" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>180</v>
+      </c>
+      <c r="H71" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>99</v>
@@ -3155,19 +3159,19 @@
         <v>22</v>
       </c>
       <c r="G72" s="2">
-        <v>210.0</v>
-      </c>
-      <c r="H72" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
+        <v>210</v>
+      </c>
+      <c r="H72" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>104</v>
@@ -3184,14 +3188,14 @@
       <c r="F73" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H73" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="74">
+      <c r="H73" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>130</v>
@@ -3209,16 +3213,16 @@
         <v>22</v>
       </c>
       <c r="G74" s="2">
-        <v>175.0</v>
-      </c>
-      <c r="H74" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>175</v>
+      </c>
+      <c r="H74" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>130</v>
@@ -3235,14 +3239,14 @@
       <c r="F75" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H75" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="76">
+      <c r="H75" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>140</v>
@@ -3260,16 +3264,16 @@
         <v>22</v>
       </c>
       <c r="G76" s="2">
-        <v>128.0</v>
-      </c>
-      <c r="H76" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="77">
+        <v>128</v>
+      </c>
+      <c r="H76" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>140</v>
@@ -3286,14 +3290,14 @@
       <c r="F77" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H77" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="78">
+      <c r="H77" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>93</v>
@@ -3311,16 +3315,16 @@
         <v>22</v>
       </c>
       <c r="G78" s="2">
-        <v>138.0</v>
-      </c>
-      <c r="H78" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>138</v>
+      </c>
+      <c r="H78" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>93</v>
@@ -3337,14 +3341,14 @@
       <c r="F79" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H79" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="80">
+      <c r="H79" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>124</v>
@@ -3362,16 +3366,16 @@
         <v>22</v>
       </c>
       <c r="G80" s="2">
-        <v>135.0</v>
-      </c>
-      <c r="H80" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="81">
+        <v>135</v>
+      </c>
+      <c r="H80" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>124</v>
@@ -3388,14 +3392,14 @@
       <c r="F81" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H81" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="82">
+      <c r="H81" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>148</v>
@@ -3413,16 +3417,16 @@
         <v>22</v>
       </c>
       <c r="G82" s="2">
-        <v>150.0</v>
-      </c>
-      <c r="H82" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="83">
+        <v>150</v>
+      </c>
+      <c r="H82" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>148</v>
@@ -3439,14 +3443,14 @@
       <c r="F83" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H83" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="84">
+      <c r="H83" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>106</v>
@@ -3464,16 +3468,16 @@
         <v>22</v>
       </c>
       <c r="G84" s="2">
-        <v>138.0</v>
-      </c>
-      <c r="H84" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="85">
+        <v>138</v>
+      </c>
+      <c r="H84" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>106</v>
@@ -3490,14 +3494,14 @@
       <c r="F85" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H85" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="86">
+      <c r="H85" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>112</v>
@@ -3515,16 +3519,16 @@
         <v>22</v>
       </c>
       <c r="G86" s="2">
-        <v>68.0</v>
-      </c>
-      <c r="H86" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="87">
+        <v>68</v>
+      </c>
+      <c r="H86" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>112</v>
@@ -3541,14 +3545,14 @@
       <c r="F87" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H87" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="88">
+      <c r="H87" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>11</v>
@@ -3560,16 +3564,16 @@
         <v>11</v>
       </c>
       <c r="G88" s="2">
-        <v>170.0</v>
-      </c>
-      <c r="H88" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>170</v>
+      </c>
+      <c r="H88" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>130</v>
@@ -3587,16 +3591,16 @@
         <v>22</v>
       </c>
       <c r="G89" s="2">
-        <v>145.0</v>
-      </c>
-      <c r="H89" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>145</v>
+      </c>
+      <c r="H89" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>130</v>
@@ -3613,14 +3617,14 @@
       <c r="F90" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H90" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="91">
+      <c r="H90" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>140</v>
@@ -3638,16 +3642,16 @@
         <v>22</v>
       </c>
       <c r="G91" s="2">
-        <v>95.0</v>
-      </c>
-      <c r="H91" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="92">
+        <v>95</v>
+      </c>
+      <c r="H91" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>140</v>
@@ -3664,14 +3668,14 @@
       <c r="F92" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H92" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="93">
+      <c r="H92" s="1" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>161</v>
@@ -3689,19 +3693,19 @@
         <v>22</v>
       </c>
       <c r="G93" s="2">
-        <v>135.0</v>
-      </c>
-      <c r="H93" s="1" t="str">
-        <f>IFS(F71:F97 = "NC",H71,F71:F97 = "Soil", "Frozen @-20*",F71:F169 = "Roller", "ETOH &amp; -20*")</f>
-        <v>ETOH &amp; -20*</v>
+        <v>135</v>
+      </c>
+      <c r="H93" s="1" t="e">
+        <f ca="1">_xludf.IFS(F71:F97 = "NC",H71,F71:F97 = "Soil", "Frozen @-20*",F71:F169 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>161</v>
@@ -3718,17 +3722,17 @@
       <c r="F94" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H94" s="1" t="str">
-        <f t="shared" ref="H94:H96" si="4">IFS(F71:F98 = "NC",H72,F71:F98 = "Soil", "Frozen @-20*",F71:F170 = "Roller", "ETOH &amp; -20*")</f>
-        <v>Frozen @-20*</v>
+      <c r="H94" s="1" t="e">
+        <f t="shared" ref="H94:H96" ca="1" si="3">_xludf.IFS(F71:F98 = "NC",H72,F71:F98 = "Soil", "Frozen @-20*",F71:F170 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>124</v>
@@ -3746,16 +3750,16 @@
         <v>22</v>
       </c>
       <c r="G95" s="2">
-        <v>165.0</v>
-      </c>
-      <c r="H95" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="96">
+        <v>165</v>
+      </c>
+      <c r="H95" s="1" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>124</v>
@@ -3772,14 +3776,14 @@
       <c r="F96" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H96" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="97">
+      <c r="H96" s="1" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>148</v>
@@ -3797,16 +3801,16 @@
         <v>22</v>
       </c>
       <c r="G97" s="2">
-        <v>105.0</v>
-      </c>
-      <c r="H97" s="1" t="str">
-        <f t="shared" ref="H97:H101" si="5">IFS(F74:F102 = "NC",H75,F74:F102 = "Soil", "Frozen @-20*",F74:F173 = "Roller", "ETOH &amp; -20*")</f>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="98">
+        <v>105</v>
+      </c>
+      <c r="H97" s="1" t="e">
+        <f t="shared" ref="H97:H101" ca="1" si="4">_xludf.IFS(F74:F102 = "NC",H75,F74:F102 = "Soil", "Frozen @-20*",F74:F173 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>148</v>
@@ -3823,14 +3827,14 @@
       <c r="F98" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H98" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="99">
+      <c r="H98" s="1" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>170</v>
@@ -3848,19 +3852,19 @@
         <v>22</v>
       </c>
       <c r="G99" s="2">
-        <v>130.0</v>
-      </c>
-      <c r="H99" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>ETOH &amp; -20*</v>
+        <v>130</v>
+      </c>
+      <c r="H99" s="1" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>170</v>
@@ -3877,17 +3881,17 @@
       <c r="F100" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H100" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>Frozen @-20*</v>
+      <c r="H100" s="1" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
-        <v>44418.0</v>
+        <v>44418</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>28</v>
@@ -3907,17 +3911,17 @@
       <c r="G101" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H101" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>#N/A</v>
+      <c r="H101" s="6" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
       </c>
       <c r="I101" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>140</v>
@@ -3935,19 +3939,19 @@
         <v>22</v>
       </c>
       <c r="G102" s="2">
-        <v>38.0</v>
-      </c>
-      <c r="H102" s="1" t="str">
-        <f t="shared" ref="H102:H123" si="6">IFS(F79:F106 = "NC",H80,F79:F106 = "Soil", "Frozen @-20*",F79:F178 = "Roller", "ETOH &amp; -20*")</f>
-        <v>ETOH &amp; -20*</v>
+        <v>38</v>
+      </c>
+      <c r="H102" s="1" t="e">
+        <f t="shared" ref="H102:H123" ca="1" si="5">_xludf.IFS(F79:F106 = "NC",H80,F79:F106 = "Soil", "Frozen @-20*",F79:F178 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>140</v>
@@ -3964,14 +3968,14 @@
       <c r="F103" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H103" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="104">
+      <c r="H103" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>148</v>
@@ -3989,16 +3993,16 @@
         <v>22</v>
       </c>
       <c r="G104" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="H104" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="105">
+        <v>50</v>
+      </c>
+      <c r="H104" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>148</v>
@@ -4015,14 +4019,14 @@
       <c r="F105" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H105" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="106">
+      <c r="H105" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>11</v>
@@ -4034,22 +4038,22 @@
         <v>11</v>
       </c>
       <c r="G106" s="2">
-        <v>82.0</v>
-      </c>
-      <c r="H106" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="107">
+        <v>82</v>
+      </c>
+      <c r="H106" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="B107" s="2">
-        <v>40.516191</v>
+        <v>40.516190999999999</v>
       </c>
       <c r="C107" s="2">
-        <v>-74.438877</v>
+        <v>-74.438877000000005</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>182</v>
@@ -4060,20 +4064,20 @@
       <c r="F107" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H107" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="108">
+      <c r="H107" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="B108" s="2">
-        <v>40.516191</v>
+        <v>40.516190999999999</v>
       </c>
       <c r="C108" s="2">
-        <v>-74.438877</v>
+        <v>-74.438877000000005</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>182</v>
@@ -4085,19 +4089,19 @@
         <v>22</v>
       </c>
       <c r="G108" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="H108" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
+        <v>20</v>
+      </c>
+      <c r="H108" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
-        <v>44420.0</v>
+        <v>44420</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>11</v>
@@ -4109,22 +4113,22 @@
         <v>11</v>
       </c>
       <c r="G109" s="2">
-        <v>62.0</v>
-      </c>
-      <c r="H109" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="110">
+        <v>62</v>
+      </c>
+      <c r="H109" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
-        <v>44420.0</v>
+        <v>44420</v>
       </c>
       <c r="B110" s="2">
-        <v>40.516191</v>
+        <v>40.516190999999999</v>
       </c>
       <c r="C110" s="2">
-        <v>-74.438877</v>
+        <v>-74.438877000000005</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>182</v>
@@ -4135,23 +4139,23 @@
       <c r="F110" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H110" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
+      <c r="H110" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
       <c r="I110" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
-        <v>44420.0</v>
+        <v>44420</v>
       </c>
       <c r="B111" s="2">
-        <v>40.516191</v>
+        <v>40.516190999999999</v>
       </c>
       <c r="C111" s="2">
-        <v>-74.438877</v>
+        <v>-74.438877000000005</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>182</v>
@@ -4163,22 +4167,22 @@
         <v>22</v>
       </c>
       <c r="G111" s="2">
-        <v>24.0</v>
-      </c>
-      <c r="H111" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="112">
+        <v>24</v>
+      </c>
+      <c r="H111" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
-        <v>44420.0</v>
+        <v>44420</v>
       </c>
       <c r="B112" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C112" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>182</v>
@@ -4189,20 +4193,20 @@
       <c r="F112" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H112" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="113">
+      <c r="H112" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
-        <v>44420.0</v>
+        <v>44420</v>
       </c>
       <c r="B113" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C113" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>182</v>
@@ -4214,19 +4218,19 @@
         <v>22</v>
       </c>
       <c r="G113" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="H113" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
+        <v>60</v>
+      </c>
+      <c r="H113" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
-        <v>44421.0</v>
+        <v>44421</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>11</v>
@@ -4238,22 +4242,22 @@
         <v>11</v>
       </c>
       <c r="G114" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="H114" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="115">
+        <v>80</v>
+      </c>
+      <c r="H114" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
-        <v>44421.0</v>
+        <v>44421</v>
       </c>
       <c r="B115" s="2">
-        <v>40.516191</v>
+        <v>40.516190999999999</v>
       </c>
       <c r="C115" s="2">
-        <v>-74.438877</v>
+        <v>-74.438877000000005</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>182</v>
@@ -4265,22 +4269,22 @@
         <v>19</v>
       </c>
       <c r="G115" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="H115" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="116">
+        <v>40</v>
+      </c>
+      <c r="H115" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
-        <v>44421.0</v>
+        <v>44421</v>
       </c>
       <c r="B116" s="2">
-        <v>40.516191</v>
+        <v>40.516190999999999</v>
       </c>
       <c r="C116" s="2">
-        <v>-74.438877</v>
+        <v>-74.438877000000005</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>182</v>
@@ -4291,20 +4295,20 @@
       <c r="F116" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H116" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="117">
+      <c r="H116" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
-        <v>44421.0</v>
+        <v>44421</v>
       </c>
       <c r="B117" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C117" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>182</v>
@@ -4316,22 +4320,22 @@
         <v>19</v>
       </c>
       <c r="G117" s="2">
-        <v>68.0</v>
-      </c>
-      <c r="H117" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="118">
+        <v>68</v>
+      </c>
+      <c r="H117" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
-        <v>44421.0</v>
+        <v>44421</v>
       </c>
       <c r="B118" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C118" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>182</v>
@@ -4342,14 +4346,14 @@
       <c r="F118" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H118" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="119">
+      <c r="H118" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
-        <v>44422.0</v>
+        <v>44422</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>11</v>
@@ -4361,22 +4365,22 @@
         <v>11</v>
       </c>
       <c r="G119" s="2">
-        <v>195.0</v>
-      </c>
-      <c r="H119" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="120">
+        <v>195</v>
+      </c>
+      <c r="H119" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
-        <v>44422.0</v>
+        <v>44422</v>
       </c>
       <c r="B120" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C120" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>182</v>
@@ -4387,20 +4391,20 @@
       <c r="F120" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H120" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="121">
+      <c r="H120" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
-        <v>44422.0</v>
+        <v>44422</v>
       </c>
       <c r="B121" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C121" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>182</v>
@@ -4412,22 +4416,22 @@
         <v>22</v>
       </c>
       <c r="G121" s="2">
-        <v>135.0</v>
-      </c>
-      <c r="H121" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="122">
+        <v>135</v>
+      </c>
+      <c r="H121" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
-        <v>44422.0</v>
+        <v>44422</v>
       </c>
       <c r="B122" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C122" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>182</v>
@@ -4438,20 +4442,20 @@
       <c r="F122" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H122" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="123">
+      <c r="H122" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
-        <v>44422.0</v>
+        <v>44422</v>
       </c>
       <c r="B123" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C123" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>182</v>
@@ -4463,16 +4467,16 @@
         <v>22</v>
       </c>
       <c r="G123" s="2">
-        <v>125.0</v>
-      </c>
-      <c r="H123" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="124">
+        <v>125</v>
+      </c>
+      <c r="H123" s="1" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A124" s="7">
-        <v>44423.0</v>
+        <v>44423</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>11</v>
@@ -4484,22 +4488,22 @@
         <v>11</v>
       </c>
       <c r="G124" s="2">
-        <v>56.0</v>
-      </c>
-      <c r="H124" s="1" t="str">
-        <f t="shared" ref="H124:H129" si="7">IFS(F102:F128 = "NC",H102,F102:F128 = "Soil", "Frozen @-20*",F102:F200 = "Roller", "ETOH &amp; -20*")</f>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="125">
+        <v>56</v>
+      </c>
+      <c r="H124" s="1" t="e">
+        <f t="shared" ref="H124:H129" ca="1" si="6">_xludf.IFS(F102:F128 = "NC",H102,F102:F128 = "Soil", "Frozen @-20*",F102:F200 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A125" s="7">
-        <v>44423.0</v>
+        <v>44423</v>
       </c>
       <c r="B125" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C125" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>182</v>
@@ -4510,20 +4514,20 @@
       <c r="F125" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H125" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="126">
+      <c r="H125" s="1" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A126" s="7">
-        <v>44423.0</v>
+        <v>44423</v>
       </c>
       <c r="B126" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C126" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>182</v>
@@ -4535,16 +4539,16 @@
         <v>22</v>
       </c>
       <c r="G126" s="2">
-        <v>34.0</v>
-      </c>
-      <c r="H126" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="127">
+        <v>34</v>
+      </c>
+      <c r="H126" s="1" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A127" s="7">
-        <v>44424.0</v>
+        <v>44424</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>11</v>
@@ -4556,22 +4560,22 @@
         <v>11</v>
       </c>
       <c r="G127" s="2">
-        <v>70.0</v>
-      </c>
-      <c r="H127" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="128">
+        <v>70</v>
+      </c>
+      <c r="H127" s="1" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A128" s="7">
-        <v>44424.0</v>
+        <v>44424</v>
       </c>
       <c r="B128" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C128" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>182</v>
@@ -4582,20 +4586,20 @@
       <c r="F128" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H128" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="129">
+      <c r="H128" s="1" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A129" s="7">
-        <v>44424.0</v>
+        <v>44424</v>
       </c>
       <c r="B129" s="2">
         <v>40.5159685</v>
       </c>
       <c r="C129" s="2">
-        <v>-74.4387762</v>
+        <v>-74.438776200000007</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>182</v>
@@ -4607,16 +4611,16 @@
         <v>22</v>
       </c>
       <c r="G129" s="2">
-        <v>44.0</v>
-      </c>
-      <c r="H129" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="130">
+        <v>44</v>
+      </c>
+      <c r="H129" s="1" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
-        <v>44452.0</v>
+        <v>44452</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>209</v>
@@ -4634,19 +4638,19 @@
         <v>22</v>
       </c>
       <c r="G130" s="2">
-        <v>54.0</v>
-      </c>
-      <c r="H130" s="1" t="str">
-        <f t="shared" ref="H130:H163" si="8">IFS(F107:F134 = "NC",H108,F107:F134 = "Soil", "Frozen @-20*",F107:F206 = "Roller", "ETOH &amp; -20*")</f>
-        <v>ETOH &amp; -20*</v>
+        <v>54</v>
+      </c>
+      <c r="H130" s="1" t="e">
+        <f t="shared" ref="H130:H163" ca="1" si="7">_xludf.IFS(F107:F134 = "NC",H108,F107:F134 = "Soil", "Frozen @-20*",F107:F206 = "Roller", "ETOH &amp; -20*")</f>
+        <v>#NAME?</v>
       </c>
       <c r="I130" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
-        <v>44452.0</v>
+        <v>44452</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>209</v>
@@ -4663,14 +4667,14 @@
       <c r="F131" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H131" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="132">
+      <c r="H131" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
-        <v>44452.0</v>
+        <v>44452</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>215</v>
@@ -4688,16 +4692,16 @@
         <v>22</v>
       </c>
       <c r="G132" s="2">
-        <v>28.0</v>
-      </c>
-      <c r="H132" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="133">
+        <v>28</v>
+      </c>
+      <c r="H132" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
-        <v>44452.0</v>
+        <v>44452</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>215</v>
@@ -4714,14 +4718,14 @@
       <c r="F133" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H133" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="134">
+      <c r="H133" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
-        <v>44452.0</v>
+        <v>44452</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>220</v>
@@ -4730,16 +4734,16 @@
         <v>11</v>
       </c>
       <c r="G134" s="2">
-        <v>102.0</v>
-      </c>
-      <c r="H134" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="135">
+        <v>102</v>
+      </c>
+      <c r="H134" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
-        <v>44453.0</v>
+        <v>44453</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>209</v>
@@ -4757,19 +4761,19 @@
         <v>22</v>
       </c>
       <c r="G135" s="2">
-        <v>12.0</v>
-      </c>
-      <c r="H135" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ETOH &amp; -20*</v>
+        <v>12</v>
+      </c>
+      <c r="H135" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
       </c>
       <c r="I135" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
-        <v>44453.0</v>
+        <v>44453</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>209</v>
@@ -4786,17 +4790,17 @@
       <c r="F136" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H136" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Frozen @-20*</v>
+      <c r="H136" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
       </c>
       <c r="I136" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
-        <v>44453.0</v>
+        <v>44453</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>215</v>
@@ -4814,16 +4818,16 @@
         <v>22</v>
       </c>
       <c r="G137" s="2">
-        <v>22.0</v>
-      </c>
-      <c r="H137" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ETOH &amp; -20*</v>
-      </c>
-    </row>
-    <row r="138">
+        <v>22</v>
+      </c>
+      <c r="H137" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
-        <v>44453.0</v>
+        <v>44453</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>215</v>
@@ -4840,14 +4844,14 @@
       <c r="F138" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H138" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="139">
+      <c r="H138" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
-        <v>44453.0</v>
+        <v>44453</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>227</v>
@@ -4856,16 +4860,16 @@
         <v>11</v>
       </c>
       <c r="G139" s="2">
-        <v>116.0</v>
-      </c>
-      <c r="H139" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="140">
+        <v>116</v>
+      </c>
+      <c r="H139" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
-        <v>44454.0</v>
+        <v>44454</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>209</v>
@@ -4883,19 +4887,19 @@
         <v>22</v>
       </c>
       <c r="G140" s="2">
-        <v>24.0</v>
-      </c>
-      <c r="H140" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ETOH &amp; -20*</v>
+        <v>24</v>
+      </c>
+      <c r="H140" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
       </c>
       <c r="I140" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
-        <v>44454.0</v>
+        <v>44454</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>209</v>
@@ -4912,14 +4916,14 @@
       <c r="F141" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H141" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="142">
+      <c r="H141" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
-        <v>44454.0</v>
+        <v>44454</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>215</v>
@@ -4937,19 +4941,19 @@
         <v>22</v>
       </c>
       <c r="G142" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="H142" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>ETOH &amp; -20*</v>
+        <v>30</v>
+      </c>
+      <c r="H142" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
       </c>
       <c r="I142" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
-        <v>44454.0</v>
+        <v>44454</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>215</v>
@@ -4966,14 +4970,14 @@
       <c r="F143" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H143" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="144">
+      <c r="H143" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
-        <v>44454.0</v>
+        <v>44454</v>
       </c>
       <c r="B144" s="4"/>
       <c r="E144" s="2" t="s">
@@ -4983,148 +4987,151 @@
         <v>11</v>
       </c>
       <c r="G144" s="2">
-        <v>100.0</v>
-      </c>
-      <c r="H144" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Frozen @-20*</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="H145" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="H146" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="H147" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="H148" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="H149" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="H150" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="H151" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="H152" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="H153" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="H154" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="H155" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="H156" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="H157" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="H158" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="H159" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="H160" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="H161" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="H162" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="H163" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>100</v>
+      </c>
+      <c r="H144" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="145" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H145" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="146" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H146" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="147" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H147" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="148" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H148" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="149" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H149" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="150" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H150" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="151" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H151" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="152" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H152" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="153" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H153" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="154" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H154" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="155" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H155" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="156" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H156" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="157" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H157" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="158" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H158" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="159" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H159" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="160" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H160" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="161" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H161" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="162" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H162" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="163" spans="8:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H163" s="1" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="36.29"/>
-    <col customWidth="1" min="3" max="3" width="22.29"/>
-    <col customWidth="1" min="4" max="4" width="81.0"/>
+    <col min="2" max="2" width="36.26953125" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="81" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>235</v>
       </c>
@@ -5147,9 +5154,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>242</v>
@@ -5161,18 +5168,18 @@
         <v>244</v>
       </c>
       <c r="E2" s="9">
-        <v>44385.0</v>
+        <v>44385</v>
       </c>
       <c r="F2" s="9">
-        <v>44386.0</v>
+        <v>44386</v>
       </c>
       <c r="G2" s="9">
-        <v>44387.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>44387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>245</v>
@@ -5184,18 +5191,18 @@
         <v>244</v>
       </c>
       <c r="E3" s="9">
-        <v>44386.0</v>
+        <v>44386</v>
       </c>
       <c r="F3" s="9">
-        <v>44387.0</v>
+        <v>44387</v>
       </c>
       <c r="G3" s="9">
-        <v>44388.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>44388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>246</v>
@@ -5207,18 +5214,18 @@
         <v>244</v>
       </c>
       <c r="E4" s="9">
-        <v>44387.0</v>
+        <v>44387</v>
       </c>
       <c r="F4" s="9">
-        <v>44388.0</v>
+        <v>44388</v>
       </c>
       <c r="G4" s="9">
-        <v>44389.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>44389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>247</v>
@@ -5230,18 +5237,18 @@
         <v>248</v>
       </c>
       <c r="E5" s="9">
-        <v>44388.0</v>
+        <v>44388</v>
       </c>
       <c r="F5" s="9">
-        <v>44389.0</v>
+        <v>44389</v>
       </c>
       <c r="G5" s="9">
-        <v>44390.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>44390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>249</v>
@@ -5253,18 +5260,18 @@
         <v>251</v>
       </c>
       <c r="E6" s="9">
-        <v>44392.0</v>
+        <v>44392</v>
       </c>
       <c r="F6" s="9">
-        <v>44393.0</v>
+        <v>44393</v>
       </c>
       <c r="G6" s="9">
-        <v>44394.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>44394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>249</v>
@@ -5276,18 +5283,18 @@
         <v>251</v>
       </c>
       <c r="E7" s="9">
-        <v>44393.0</v>
+        <v>44393</v>
       </c>
       <c r="F7" s="9">
-        <v>44393.0</v>
+        <v>44393</v>
       </c>
       <c r="G7" s="9">
-        <v>44394.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>44394</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>252</v>
@@ -5299,18 +5306,18 @@
         <v>253</v>
       </c>
       <c r="E8" s="9">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="F8" s="9">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="G8" s="9">
-        <v>44416.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>44416</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>254</v>
@@ -5322,18 +5329,18 @@
         <v>255</v>
       </c>
       <c r="E9" s="9">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="F9" s="9">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="G9" s="9">
-        <v>44416.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>44416</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>256</v>
@@ -5345,18 +5352,18 @@
         <v>257</v>
       </c>
       <c r="E10" s="9">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="F10" s="9">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="G10" s="9">
-        <v>44416.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>44416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>258</v>
@@ -5368,18 +5375,18 @@
         <v>257</v>
       </c>
       <c r="E11" s="9">
-        <v>44414.0</v>
+        <v>44414</v>
       </c>
       <c r="F11" s="9">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="G11" s="9">
-        <v>44416.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>44416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>259</v>
@@ -5391,18 +5398,18 @@
         <v>253</v>
       </c>
       <c r="E12" s="9">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="F12" s="9">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="G12" s="9">
-        <v>44417.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>44417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>260</v>
@@ -5414,18 +5421,18 @@
         <v>255</v>
       </c>
       <c r="E13" s="9">
-        <v>44415.0</v>
+        <v>44415</v>
       </c>
       <c r="F13" s="9">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="G13" s="9">
-        <v>44417.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>44417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>261</v>
@@ -5437,18 +5444,18 @@
         <v>255</v>
       </c>
       <c r="E14" s="9">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="F14" s="9">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="G14" s="9">
-        <v>44419.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>44419</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>262</v>
@@ -5460,18 +5467,18 @@
         <v>253</v>
       </c>
       <c r="E15" s="9">
-        <v>44416.0</v>
+        <v>44416</v>
       </c>
       <c r="F15" s="9">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="G15" s="9">
-        <v>44419.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>44419</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>263</v>
@@ -5483,18 +5490,18 @@
         <v>264</v>
       </c>
       <c r="E16" s="9">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="F16" s="9">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="G16" s="9">
-        <v>44420.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>44420</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>265</v>
@@ -5506,18 +5513,18 @@
         <v>266</v>
       </c>
       <c r="E17" s="9">
-        <v>44417.0</v>
+        <v>44417</v>
       </c>
       <c r="F17" s="9">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="G17" s="9">
-        <v>44420.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>44420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>267</v>
@@ -5529,18 +5536,18 @@
         <v>268</v>
       </c>
       <c r="E18" s="9">
-        <v>44419.0</v>
+        <v>44419</v>
       </c>
       <c r="F18" s="9">
-        <v>44420.0</v>
+        <v>44420</v>
       </c>
       <c r="G18" s="9">
-        <v>44421.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>44421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>269</v>
@@ -5552,18 +5559,18 @@
         <v>268</v>
       </c>
       <c r="E19" s="9">
-        <v>44420.0</v>
+        <v>44420</v>
       </c>
       <c r="F19" s="9">
-        <v>44421.0</v>
+        <v>44421</v>
       </c>
       <c r="G19" s="9">
-        <v>44422.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>44422</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>269</v>
@@ -5575,18 +5582,18 @@
         <v>268</v>
       </c>
       <c r="E20" s="9">
-        <v>44422.0</v>
+        <v>44422</v>
       </c>
       <c r="F20" s="9">
-        <v>44423.0</v>
+        <v>44423</v>
       </c>
       <c r="G20" s="9">
-        <v>44424.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>44424</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>19.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>270</v>
@@ -5598,18 +5605,18 @@
         <v>211</v>
       </c>
       <c r="E21" s="9">
-        <v>44452.0</v>
+        <v>44452</v>
       </c>
       <c r="F21" s="9">
-        <v>44453.0</v>
+        <v>44453</v>
       </c>
       <c r="G21" s="9">
-        <v>44454.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>44454</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>20.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>271</v>
@@ -5621,40 +5628,41 @@
         <v>217</v>
       </c>
       <c r="E22" s="9">
-        <v>44452.0</v>
+        <v>44452</v>
       </c>
       <c r="F22" s="9">
-        <v>44453.0</v>
+        <v>44453</v>
       </c>
       <c r="G22" s="9">
-        <v>44454.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>44454</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.14"/>
-    <col customWidth="1" min="2" max="2" width="86.29"/>
-    <col customWidth="1" min="3" max="3" width="33.57"/>
-    <col customWidth="1" min="4" max="4" width="22.0"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
+    <col min="2" max="2" width="86.26953125" customWidth="1"/>
+    <col min="3" max="3" width="33.54296875" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>272</v>
       </c>
@@ -5663,7 +5671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>273</v>
       </c>
@@ -5671,7 +5679,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>275</v>
       </c>
@@ -5685,7 +5693,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>278</v>
       </c>
@@ -5699,12 +5707,12 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>281</v>
       </c>
@@ -5712,7 +5720,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>283</v>
       </c>
@@ -5720,7 +5728,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>285</v>
       </c>
@@ -5728,7 +5736,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>287</v>
       </c>
@@ -5737,27 +5745,27 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.14"/>
-    <col customWidth="1" min="2" max="2" width="32.43"/>
-    <col customWidth="1" min="7" max="7" width="15.71"/>
+    <col min="1" max="1" width="10.08984375" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
@@ -5785,9 +5793,8 @@
       <c r="I1" s="14"/>
     </row>
   </sheetData>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>